<commit_message>
with Vader code commented here
</commit_message>
<xml_diff>
--- a/regression_results.xlsx
+++ b/regression_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,22 +487,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-90.35865196042599</v>
+        <v>-43.8252333487047</v>
       </c>
       <c r="D2" t="n">
-        <v>1.451725599164051e-15</v>
+        <v>0.03285282928370578</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="3">
@@ -517,22 +517,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.04565161843321153</v>
+        <v>0.02362618538139191</v>
       </c>
       <c r="D3" t="n">
-        <v>4.377308476365676e-16</v>
+        <v>0.02037410306100642</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="4">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1203485161460133</v>
+        <v>0.3891309111991351</v>
       </c>
       <c r="D4" t="n">
-        <v>8.856279548591782e-12</v>
+        <v>1.019440973731556e-23</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="5">
@@ -577,22 +577,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.002225252698696348</v>
+        <v>0.006769402093940205</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001027593195668259</v>
+        <v>4.288545333344304e-08</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="6">
@@ -607,22 +607,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.007586752400305641</v>
+        <v>0.06353883292422918</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001449434449709041</v>
+        <v>2.353804242694394e-21</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="7">
@@ -637,22 +637,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.01498130454042387</v>
+        <v>0.1218990873078701</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7306874546766906</v>
+        <v>0.1223873254900664</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="8">
@@ -667,22 +667,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.06799552572882885</v>
+        <v>-0.02462753093527517</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08909891023851452</v>
+        <v>0.7352825019571567</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="9">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.07360785484831146</v>
+        <v>-0.6714849375736641</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1646993356957894</v>
+        <v>3.838930075153281e-12</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="10">
@@ -727,22 +727,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02971136139410686</v>
+        <v>-0.116107062659266</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4308049712924823</v>
+        <v>0.09189021232048347</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="11">
@@ -757,22 +757,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1109558865633706</v>
+        <v>0.4717506508983828</v>
       </c>
       <c r="D11" t="n">
-        <v>0.03575034476270502</v>
+        <v>9.619713999603922e-07</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="12">
@@ -787,22 +787,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.04427415731452759</v>
+        <v>0.5312788849591763</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3587811587238802</v>
+        <v>1.796318178140144e-09</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="13">
@@ -817,22 +817,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1073344050175514</v>
+        <v>-0.3002566725303573</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02900064687318418</v>
+        <v>0.0008178513884850787</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="14">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.1711834270791853</v>
+        <v>0.4604889734022516</v>
       </c>
       <c r="D14" t="n">
-        <v>8.400473750280077e-07</v>
+        <v>3.621381104698225e-13</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="15">
@@ -877,22 +877,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.2978380793392251</v>
+        <v>0.740535880491475</v>
       </c>
       <c r="D15" t="n">
-        <v>5.332050345127606e-10</v>
+        <v>1.643218334867517e-17</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="16">
@@ -907,22 +907,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.05237330572188882</v>
+        <v>0.1716332612165648</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1610128763790879</v>
+        <v>0.01177912543282537</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H16" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="17">
@@ -937,22 +937,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.1840956799547261</v>
+        <v>-1.012376435441653</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1420625958982232</v>
+        <v>0.01425548237235368</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H17" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="18">
@@ -967,22 +967,22 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1323767387381435</v>
+        <v>0.07035145876140922</v>
       </c>
       <c r="D18" t="n">
-        <v>0.005237192014002194</v>
+        <v>0.008625544325999168</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="19">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.905026761878961e-06</v>
+        <v>-0.008812991728604653</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5526190429441227</v>
+        <v>0.3211047679285141</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H19" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="20">
@@ -1027,22 +1027,22 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-3.559337492002851</v>
+        <v>2.339502210442216</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4227227960224119</v>
+        <v>0.5413028639566368</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G20" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="21">
@@ -1057,22 +1057,22 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.2120488747052436</v>
+        <v>-0.04788207345458586</v>
       </c>
       <c r="D21" t="n">
-        <v>0.07870757103545929</v>
+        <v>0.8280903833998621</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="22">
@@ -1087,22 +1087,22 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.03586979435216319</v>
+        <v>-0.1069903726951685</v>
       </c>
       <c r="D22" t="n">
-        <v>2.712197968332279e-05</v>
+        <v>9.058533046428861e-12</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="23">
@@ -1117,22 +1117,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.3003162644560166</v>
+        <v>0.06733083444275073</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2098803688679735</v>
+        <v>0.8774929985221944</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="24">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.09346855149774624</v>
+        <v>-0.7121430658814929</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7508875763409334</v>
+        <v>0.1846024448225281</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H24" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="25">
@@ -1177,22 +1177,22 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5553583091700669</v>
+        <v>0.6661142237900112</v>
       </c>
       <c r="D25" t="n">
-        <v>0.07348085225904095</v>
+        <v>0.2386291171570335</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="26">
@@ -1207,22 +1207,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.306352679780713</v>
+        <v>0.7402135422236131</v>
       </c>
       <c r="D26" t="n">
-        <v>0.269820978003532</v>
+        <v>0.1439308837834031</v>
       </c>
       <c r="E26" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G26" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H26" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="27">
@@ -1237,22 +1237,22 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-2.87396162260801</v>
+        <v>-0.110647385359129</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0098136032326691</v>
+        <v>0.9774868025276635</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G27" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H27" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="28">
@@ -1267,22 +1267,22 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>11.31977239894125</v>
+        <v>230.4003120814403</v>
       </c>
       <c r="D28" t="n">
-        <v>0.04927410971866649</v>
+        <v>0.2514330054216104</v>
       </c>
       <c r="E28" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G28" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H28" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="29">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.06051524034283562</v>
+        <v>0.1483252544924223</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7224570669157653</v>
+        <v>0.6331107975981328</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G29" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H29" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="30">
@@ -1327,22 +1327,22 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-2.857512425553223</v>
+        <v>0.09220587816716463</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03097192004313973</v>
+        <v>0.9892179180608173</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G30" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H30" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="31">
@@ -1357,22 +1357,22 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.5237553069806544</v>
+        <v>-1.064911857949007</v>
       </c>
       <c r="D31" t="n">
-        <v>0.03208330911989713</v>
+        <v>0.4277533955382481</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="32">
@@ -1387,22 +1387,22 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.6624755346153468</v>
+        <v>2.487039094084162</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1054651049980036</v>
+        <v>0.05988240896943365</v>
       </c>
       <c r="E32" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G32" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H32" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
       </c>
     </row>
     <row r="33">
@@ -1417,22 +1417,472 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.3843461889965976</v>
+        <v>0.8099952688434624</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4066934173388453</v>
+        <v>0.579017715115594</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2003978947046451</v>
+        <v>0.4412257720869083</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1896018732481312</v>
+        <v>0.4337658233077069</v>
       </c>
       <c r="G33" t="n">
-        <v>0.3622978580100727</v>
+        <v>1.216707847767516</v>
       </c>
       <c r="H33" t="n">
-        <v>0.4792987473408266</v>
+        <v>0.8807848215939169</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>-40.98164797904721</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.04162042136235278</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>TrailerPublishYear</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.02030642471571845</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0416704482270633</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TrailerPublishDays</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.3900458181078471</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.720484303159662e-23</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>TrailerDuration</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0.008232302159308843</v>
+      </c>
+      <c r="D37" t="n">
+        <v>5.327214001419852e-16</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ProductionBudget</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.06859348883087343</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.201541555368325e-24</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.1492002496941142</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0526721806325547</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Comedy</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.02010186390894747</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.766070962337832</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Documentary</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.6582390124252219</v>
+      </c>
+      <c r="D41" t="n">
+        <v>6.719795663874087e-13</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.1030218627816445</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.1324395214722167</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.4946225307248153</v>
+      </c>
+      <c r="D43" t="n">
+        <v>3.662215626930061e-07</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.5400133408287348</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.352137861142645e-09</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Not Rated</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.3236089438349208</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.000339126620250968</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TopStars</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.4188153081035941</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4.359940702255215e-11</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TopStudios</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0.7557257309017842</v>
+      </c>
+      <c r="D47" t="n">
+        <v>5.742208729394474e-18</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.8959622673844697</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>cont</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ProductionCountry</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.1484980106232207</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.03009809895157389</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.4226810072822857</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.4192254853079171</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1.257088308686512</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.8959622673844697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>